<commit_message>
update egg notes EGK
</commit_message>
<xml_diff>
--- a/Data/Processed/egg_notes_EGK.xlsx
+++ b/Data/Processed/egg_notes_EGK.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethking/Dropbox/WORK/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kingeg/Documents/h2lifespan/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
   <si>
     <t>Image</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>no eggs</t>
+  </si>
+  <si>
+    <t>some food</t>
   </si>
 </sst>
 </file>
@@ -368,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,6 +707,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1875</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2525</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2413</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2017</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1913</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1880</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2528</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1983</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
R script added, egg notes updated
</commit_message>
<xml_diff>
--- a/Data/Processed/egg_notes_EGK.xlsx
+++ b/Data/Processed/egg_notes_EGK.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kingeg/Documents/h2lifespan/Data/Processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/h2lifespan/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16520" yWindow="460" windowWidth="12280" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="6140" yWindow="460" windowWidth="14560" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>Image</t>
   </si>
@@ -57,6 +57,54 @@
   </si>
   <si>
     <t>some food</t>
+  </si>
+  <si>
+    <t>IMG_1880.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2049.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2124.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2137.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2139.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2142.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2178.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2525.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2528.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2822.JPG</t>
+  </si>
+  <si>
+    <t>IMG_2921.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3035.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3056.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3085.JPG</t>
+  </si>
+  <si>
+    <t>IMG_3442.JPG</t>
+  </si>
+  <si>
+    <t>Bad_thresh</t>
   </si>
 </sst>
 </file>
@@ -371,13 +419,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -389,47 +440,47 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2043</v>
+        <v>1875</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2239</v>
+        <v>1880</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3340</v>
+        <v>1913</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2375</v>
+        <v>1983</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2373</v>
+        <v>2017</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2372</v>
+        <v>2043</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -437,7 +488,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2469</v>
+        <v>2239</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -445,7 +496,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2588</v>
+        <v>2372</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -453,7 +504,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2691</v>
+        <v>2373</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -461,7 +512,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2756</v>
+        <v>2375</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -469,39 +520,39 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2751</v>
+        <v>2413</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2822</v>
+        <v>2469</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2858</v>
+        <v>2525</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2857</v>
+        <v>2528</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2859</v>
+        <v>2588</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -509,7 +560,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2860</v>
+        <v>2691</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -517,15 +568,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2899</v>
+        <v>2751</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2898</v>
+        <v>2756</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -533,15 +584,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2916</v>
+        <v>2822</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2938</v>
+        <v>2857</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -549,31 +600,31 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2935</v>
+        <v>2858</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2934</v>
+        <v>2859</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2933</v>
+        <v>2860</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>3102</v>
+        <v>2898</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -581,7 +632,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>3349</v>
+        <v>2899</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -589,58 +640,58 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>3320</v>
+        <v>2916</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>3319</v>
+        <v>2933</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>3318</v>
+        <v>2934</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>3317</v>
+        <v>2935</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>3316</v>
+        <v>2938</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>3247</v>
+        <v>3085</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>3234</v>
+        <v>3102</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -653,7 +704,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>3085</v>
+        <v>3234</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
@@ -661,117 +712,200 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>3565</v>
+        <v>3247</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>3602</v>
+        <v>3316</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>3601</v>
+        <v>3317</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>3679</v>
+        <v>3318</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>3663</v>
+        <v>3319</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>3840</v>
+        <v>3320</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1875</v>
+        <v>3340</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2525</v>
+        <v>3349</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>2413</v>
+        <v>3565</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>2017</v>
+        <v>3601</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>1913</v>
+        <v>3602</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>1880</v>
+        <v>3663</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>2528</v>
+        <v>3679</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>1983</v>
+        <v>3840</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B49">
+    <sortCondition ref="A2:A49"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data added to egg notes
</commit_message>
<xml_diff>
--- a/Data/Processed/egg_notes_EGK.xlsx
+++ b/Data/Processed/egg_notes_EGK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="1740" windowWidth="21160" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="12080" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,6 +310,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -335,11 +341,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -623,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1168,6 +1175,9 @@
       <c r="A49" t="s">
         <v>23</v>
       </c>
+      <c r="B49">
+        <v>985</v>
+      </c>
       <c r="C49" t="s">
         <v>4</v>
       </c>
@@ -1187,6 +1197,9 @@
       <c r="A51" t="s">
         <v>54</v>
       </c>
+      <c r="B51" s="1">
+        <v>631</v>
+      </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
@@ -1195,6 +1208,9 @@
       <c r="A52" t="s">
         <v>55</v>
       </c>
+      <c r="B52" s="4">
+        <v>572</v>
+      </c>
       <c r="C52" t="s">
         <v>4</v>
       </c>
@@ -1203,6 +1219,9 @@
       <c r="A53" t="s">
         <v>56</v>
       </c>
+      <c r="B53" s="4">
+        <v>409</v>
+      </c>
       <c r="C53" t="s">
         <v>4</v>
       </c>
@@ -1210,6 +1229,9 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
+      </c>
+      <c r="B54">
+        <v>613</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
hand counts added to egg notes
</commit_message>
<xml_diff>
--- a/Data/Processed/egg_notes_EGK.xlsx
+++ b/Data/Processed/egg_notes_EGK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="12080" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="16400" yWindow="3220" windowWidth="12080" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="77">
   <si>
     <t>Image</t>
   </si>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,8 +748,8 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>74</v>
+      <c r="B8">
+        <v>224</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1003,6 +1003,9 @@
       <c r="A29" t="s">
         <v>38</v>
       </c>
+      <c r="B29">
+        <v>715</v>
+      </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
@@ -1011,6 +1014,9 @@
       <c r="A30" t="s">
         <v>40</v>
       </c>
+      <c r="B30">
+        <v>120</v>
+      </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
@@ -1019,6 +1025,9 @@
       <c r="A31" t="s">
         <v>41</v>
       </c>
+      <c r="B31">
+        <v>830</v>
+      </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
@@ -1035,6 +1044,9 @@
       <c r="A33" t="s">
         <v>19</v>
       </c>
+      <c r="B33">
+        <v>157</v>
+      </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
@@ -1054,6 +1066,9 @@
       <c r="A35" t="s">
         <v>43</v>
       </c>
+      <c r="B35">
+        <v>853</v>
+      </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
@@ -1062,6 +1077,9 @@
       <c r="A36" t="s">
         <v>44</v>
       </c>
+      <c r="B36">
+        <v>526</v>
+      </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
@@ -1070,6 +1088,9 @@
       <c r="A37" t="s">
         <v>45</v>
       </c>
+      <c r="B37">
+        <v>195</v>
+      </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
@@ -1078,6 +1099,9 @@
       <c r="A38" t="s">
         <v>46</v>
       </c>
+      <c r="B38">
+        <v>368</v>
+      </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
@@ -1086,6 +1110,9 @@
       <c r="A39" t="s">
         <v>47</v>
       </c>
+      <c r="B39">
+        <v>338</v>
+      </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
@@ -1094,6 +1121,9 @@
       <c r="A40" t="s">
         <v>48</v>
       </c>
+      <c r="B40">
+        <v>85</v>
+      </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
@@ -1102,6 +1132,9 @@
       <c r="A41" t="s">
         <v>49</v>
       </c>
+      <c r="B41">
+        <v>647</v>
+      </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
@@ -1121,6 +1154,9 @@
       <c r="A43" t="s">
         <v>50</v>
       </c>
+      <c r="B43">
+        <v>841</v>
+      </c>
       <c r="C43" t="s">
         <v>5</v>
       </c>
@@ -1129,6 +1165,9 @@
       <c r="A44" t="s">
         <v>51</v>
       </c>
+      <c r="B44">
+        <v>770</v>
+      </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
@@ -1137,6 +1176,9 @@
       <c r="A45" t="s">
         <v>52</v>
       </c>
+      <c r="B45">
+        <v>747</v>
+      </c>
       <c r="C45" t="s">
         <v>5</v>
       </c>
@@ -1144,6 +1186,9 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
+      </c>
+      <c r="B46">
+        <v>326</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
added egg counts to notes
</commit_message>
<xml_diff>
--- a/Data/Processed/egg_notes_EGK.xlsx
+++ b/Data/Processed/egg_notes_EGK.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16400" yWindow="3220" windowWidth="12080" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="16180" yWindow="2160" windowWidth="12080" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,6 +971,9 @@
       <c r="A25" t="s">
         <v>33</v>
       </c>
+      <c r="B25" s="4">
+        <v>401</v>
+      </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
@@ -979,6 +982,9 @@
       <c r="A26" t="s">
         <v>34</v>
       </c>
+      <c r="B26" s="4">
+        <v>1578</v>
+      </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
@@ -987,6 +993,9 @@
       <c r="A27" t="s">
         <v>35</v>
       </c>
+      <c r="B27" s="4">
+        <v>819</v>
+      </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
@@ -995,6 +1004,9 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
+      <c r="B28" s="4">
+        <v>425</v>
+      </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
@@ -1035,6 +1047,9 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>42</v>
+      </c>
+      <c r="B32">
+        <v>1065</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>

</xml_diff>